<commit_message>
[AETF]: Excel Report Template file updated.
</commit_message>
<xml_diff>
--- a/Automated_ECU_Test_Framework/Libs/report/reportTLA.xlsx
+++ b/Automated_ECU_Test_Framework/Libs/report/reportTLA.xlsx
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,12 +133,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -237,30 +231,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -270,23 +242,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -301,88 +291,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_CW170-DVP&amp;SOR" xfId="1"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1195,7 +1104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1204,281 +1113,224 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="52.33203125" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="10" customWidth="1"/>
     <col min="9" max="9" width="44.109375" customWidth="1"/>
     <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="17" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="13">
         <f>COUNTIF(H13:H1048576,"OK")</f>
         <v>0</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="13">
         <f>COUNTIF(H13:H1048576,"NOK")</f>
         <v>0</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:15" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
+    <row r="11" spans="1:9" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:15" s="9" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" s="3" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="H13:H1048576">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",H13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:I1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A13="TS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$A13="TH"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A13:A16">
-      <formula1>"TH,TS"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>